<commit_message>
Updated for Velocity's DDGs
</commit_message>
<xml_diff>
--- a/velocity_template.xlsx
+++ b/velocity_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repo\touch_DDGs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908A8F65-5F0B-4B00-A4D8-DD981AAC6F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E0FC95-CBC4-4761-9349-657443785AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7260" yWindow="1710" windowWidth="28800" windowHeight="11385" xr2:uid="{4C7E114B-A30A-4DC9-9FF5-1565BE38942B}"/>
+    <workbookView xWindow="16680" yWindow="3975" windowWidth="57600" windowHeight="15435" xr2:uid="{4C7E114B-A30A-4DC9-9FF5-1565BE38942B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Group</t>
   </si>
@@ -42,12 +42,6 @@
     <t>Alias</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -72,16 +66,16 @@
     <t>teknomageemployees</t>
   </si>
   <si>
-    <t>teknomageaustinallstaff</t>
-  </si>
-  <si>
-    <t>teknomageaustinemployees</t>
-  </si>
-  <si>
     <t>Bluffton</t>
   </si>
   <si>
-    <t>SC</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>teknomageblufftonallstaff</t>
+  </si>
+  <si>
+    <t>teknomagblufftonemployees</t>
   </si>
 </sst>
 </file>
@@ -433,87 +427,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDAF3DBB-E1DD-4AD4-A78C-3C0BF173F495}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="A1:D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated for new Vleocity DDGs
</commit_message>
<xml_diff>
--- a/velocity_template.xlsx
+++ b/velocity_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repo\touch_DDGs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E0FC95-CBC4-4761-9349-657443785AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835EE7E7-8777-489D-9006-02FFFA382B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="3975" windowWidth="57600" windowHeight="15435" xr2:uid="{4C7E114B-A30A-4DC9-9FF5-1565BE38942B}"/>
+    <workbookView xWindow="44160" yWindow="1800" windowWidth="28995" windowHeight="15435" xr2:uid="{4C7E114B-A30A-4DC9-9FF5-1565BE38942B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="134">
   <si>
     <t>Group</t>
   </si>
@@ -48,34 +48,394 @@
     <t>Employee</t>
   </si>
   <si>
-    <t>Teknomage All Staff</t>
-  </si>
-  <si>
-    <t>Teknomage Employees</t>
-  </si>
-  <si>
-    <t>Teknomage Bluffton All Staff</t>
-  </si>
-  <si>
-    <t>Teknomage Bluffton Employees</t>
-  </si>
-  <si>
-    <t>teknomageallstaff</t>
-  </si>
-  <si>
-    <t>teknomageemployees</t>
-  </si>
-  <si>
-    <t>Bluffton</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>teknomageblufftonallstaff</t>
-  </si>
-  <si>
-    <t>teknomagblufftonemployees</t>
+    <t>Velocity All Staff</t>
+  </si>
+  <si>
+    <t>velocityallstaff</t>
+  </si>
+  <si>
+    <t>Velocity Employees</t>
+  </si>
+  <si>
+    <t>velocityemployees</t>
+  </si>
+  <si>
+    <t>velocityandersonallstaff</t>
+  </si>
+  <si>
+    <t>velocityandersonemployees</t>
+  </si>
+  <si>
+    <t>Velocity Anderson All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Anderson Employees</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Velocity Austin All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Austin Employees</t>
+  </si>
+  <si>
+    <t>velocityaustinallstaff</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>Banning</t>
+  </si>
+  <si>
+    <t>Boise</t>
+  </si>
+  <si>
+    <t>Chula Vista</t>
+  </si>
+  <si>
+    <t>Cincinatti</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
+  </si>
+  <si>
+    <t>velocityaustinemployees</t>
+  </si>
+  <si>
+    <t>Columbia</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Gaffney</t>
+  </si>
+  <si>
+    <t>Grants Pass</t>
+  </si>
+  <si>
+    <t>Greenville</t>
+  </si>
+  <si>
+    <t>Hallandale Beach</t>
+  </si>
+  <si>
+    <t>HQ</t>
+  </si>
+  <si>
+    <t>Medford</t>
+  </si>
+  <si>
+    <t>New Smyrna Beach</t>
+  </si>
+  <si>
+    <t>North Hollywood</t>
+  </si>
+  <si>
+    <t>Providence</t>
+  </si>
+  <si>
+    <t>Salt Lake City</t>
+  </si>
+  <si>
+    <t>San Diego</t>
+  </si>
+  <si>
+    <t>Spartanburg</t>
+  </si>
+  <si>
+    <t>Spokane</t>
+  </si>
+  <si>
+    <t>Syracuse</t>
+  </si>
+  <si>
+    <t>Union</t>
+  </si>
+  <si>
+    <t>Valparaiso</t>
+  </si>
+  <si>
+    <t>Velocity Banning All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Boise All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Chula Vista All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Cincinatti All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Cleveland All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Columbia All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Denver All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Gaffney All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Grants Pass All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Greenville All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Hallandale Beach All Staff</t>
+  </si>
+  <si>
+    <t>Velocity HQ All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Medford All Staff</t>
+  </si>
+  <si>
+    <t>Velocity New Smyrna Beach All Staff</t>
+  </si>
+  <si>
+    <t>Velocity North Hollywood All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Banning Employees</t>
+  </si>
+  <si>
+    <t>Velocity Boise Employees</t>
+  </si>
+  <si>
+    <t>Velocity Chula Vista Employees</t>
+  </si>
+  <si>
+    <t>Velocity Cincinatti Employees</t>
+  </si>
+  <si>
+    <t>Velocity Cleveland Employees</t>
+  </si>
+  <si>
+    <t>Velocity Columbia Employees</t>
+  </si>
+  <si>
+    <t>Velocity Denver Employees</t>
+  </si>
+  <si>
+    <t>Velocity Gaffney Employees</t>
+  </si>
+  <si>
+    <t>Velocity Grants Pass Employees</t>
+  </si>
+  <si>
+    <t>Velocity Greenville Employees</t>
+  </si>
+  <si>
+    <t>Velocity Hallandale Beach Employees</t>
+  </si>
+  <si>
+    <t>Velocity HQ Employees</t>
+  </si>
+  <si>
+    <t>Velocity Medford Employees</t>
+  </si>
+  <si>
+    <t>Velocity New Smyrna Beach Employees</t>
+  </si>
+  <si>
+    <t>Velocity North Hollywood Employees</t>
+  </si>
+  <si>
+    <t>velocitybanningallstaff</t>
+  </si>
+  <si>
+    <t>velocitybanningemployees</t>
+  </si>
+  <si>
+    <t>Velocity Providence All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Providence Employees</t>
+  </si>
+  <si>
+    <t>Velocity Salt Lake City All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Salt Lake City Employees</t>
+  </si>
+  <si>
+    <t>Velocity San Diego All Staff</t>
+  </si>
+  <si>
+    <t>Velocity San Diego Employees</t>
+  </si>
+  <si>
+    <t>Velocity Spartanburg All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Spartanburg Employees</t>
+  </si>
+  <si>
+    <t>Velocity Spokane All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Spokane Employees</t>
+  </si>
+  <si>
+    <t>Velocity Syracuse All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Syracuse Employees</t>
+  </si>
+  <si>
+    <t>Velocity Union All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Union Employees</t>
+  </si>
+  <si>
+    <t>Velocity Valparaiso All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Valparaiso Employees</t>
+  </si>
+  <si>
+    <t>velocityboiseallstaff</t>
+  </si>
+  <si>
+    <t>velocityboiseemployees</t>
+  </si>
+  <si>
+    <t>velocitychulavistaallstaff</t>
+  </si>
+  <si>
+    <t>velocitychulavistaemployees</t>
+  </si>
+  <si>
+    <t>velocitycincinattiallstaff</t>
+  </si>
+  <si>
+    <t>velocitycincinattiemployees</t>
+  </si>
+  <si>
+    <t>velocityclevelandallstaff</t>
+  </si>
+  <si>
+    <t>velocityclevelandemployees</t>
+  </si>
+  <si>
+    <t>velocitycolumbiaallstaff</t>
+  </si>
+  <si>
+    <t>velocitycolumbiaemployees</t>
+  </si>
+  <si>
+    <t>velocitydenverallstaff</t>
+  </si>
+  <si>
+    <t>velocitydenveremployees</t>
+  </si>
+  <si>
+    <t>velocitygaffneyallstaff</t>
+  </si>
+  <si>
+    <t>velocitygaffneyemployees</t>
+  </si>
+  <si>
+    <t>velocitygrantspassallstaff</t>
+  </si>
+  <si>
+    <t>velocitygrantspassemployees</t>
+  </si>
+  <si>
+    <t>velocitygreenvilleallstaff</t>
+  </si>
+  <si>
+    <t>velocitygreenvilleemployees</t>
+  </si>
+  <si>
+    <t>velocityhallandalebeachallstaff</t>
+  </si>
+  <si>
+    <t>velocityhallandalebeachemployees</t>
+  </si>
+  <si>
+    <t>velocityhqallstaff</t>
+  </si>
+  <si>
+    <t>velocityhqemployees</t>
+  </si>
+  <si>
+    <t>velocitymedfordallstaff</t>
+  </si>
+  <si>
+    <t>velocitymedfordemployees</t>
+  </si>
+  <si>
+    <t>velocitynewsmyrnabeachallstaff</t>
+  </si>
+  <si>
+    <t>velocitynewsmyrnabeachemployees</t>
+  </si>
+  <si>
+    <t>velocitynorthhollywoodallstaff</t>
+  </si>
+  <si>
+    <t>velocitynorthhollywoodemployees</t>
+  </si>
+  <si>
+    <t>velocityprovidenceallstaff</t>
+  </si>
+  <si>
+    <t>velocityprovidenceemployees</t>
+  </si>
+  <si>
+    <t>velocitysaltlakecityallstaff</t>
+  </si>
+  <si>
+    <t>velocitysaltlakecityemployees</t>
+  </si>
+  <si>
+    <t>velocitysandiegoallstaff</t>
+  </si>
+  <si>
+    <t>velocitysandiegoemployees</t>
+  </si>
+  <si>
+    <t>velocityspartanburgallstaff</t>
+  </si>
+  <si>
+    <t>velocityspartanburgemployees</t>
+  </si>
+  <si>
+    <t>velocityspokaneallstaff</t>
+  </si>
+  <si>
+    <t>velocityspokaneemployees</t>
+  </si>
+  <si>
+    <t>velocitysyracuseallstaff</t>
+  </si>
+  <si>
+    <t>velocitysyracuseemployees</t>
+  </si>
+  <si>
+    <t>velocityunionallstaff</t>
+  </si>
+  <si>
+    <t>velocityunionemployees</t>
+  </si>
+  <si>
+    <t>velocityvalparaisoallstaff</t>
+  </si>
+  <si>
+    <t>velocityvalparaisoemployees</t>
   </si>
 </sst>
 </file>
@@ -427,23 +787,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDAF3DBB-E1DD-4AD4-A78C-3C0BF173F495}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="A1:D5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -457,18 +817,18 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -476,26 +836,626 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
       <c r="D5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" t="s">
+        <v>125</v>
+      </c>
+      <c r="C45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" t="s">
+        <v>126</v>
+      </c>
+      <c r="C46" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" t="s">
+        <v>130</v>
+      </c>
+      <c r="C50" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>87</v>
+      </c>
+      <c r="B51" t="s">
+        <v>131</v>
+      </c>
+      <c r="C51" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53" t="s">
+        <v>133</v>
+      </c>
+      <c r="C53" t="s">
+        <v>41</v>
+      </c>
+      <c r="D53" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Selections per Velocity Choices
</commit_message>
<xml_diff>
--- a/velocity_template.xlsx
+++ b/velocity_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repo\touch_DDGs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835EE7E7-8777-489D-9006-02FFFA382B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F694BAD3-F6FE-49B1-AA8B-C4FE54F21BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44160" yWindow="1800" windowWidth="28995" windowHeight="15435" xr2:uid="{4C7E114B-A30A-4DC9-9FF5-1565BE38942B}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="57600" windowHeight="15435" xr2:uid="{4C7E114B-A30A-4DC9-9FF5-1565BE38942B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -99,9 +99,6 @@
     <t>Chula Vista</t>
   </si>
   <si>
-    <t>Cincinatti</t>
-  </si>
-  <si>
     <t>Cleveland</t>
   </si>
   <si>
@@ -318,12 +315,6 @@
     <t>velocitychulavistaemployees</t>
   </si>
   <si>
-    <t>velocitycincinattiallstaff</t>
-  </si>
-  <si>
-    <t>velocitycincinattiemployees</t>
-  </si>
-  <si>
     <t>velocityclevelandallstaff</t>
   </si>
   <si>
@@ -436,6 +427,15 @@
   </si>
   <si>
     <t>velocityvalparaisoemployees</t>
+  </si>
+  <si>
+    <t>Cincinnati</t>
+  </si>
+  <si>
+    <t>velocitycincinnatiallstaff</t>
+  </si>
+  <si>
+    <t>velocitycincinnatiemployees</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,7 +875,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -886,10 +886,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -897,10 +897,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -911,10 +911,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -922,10 +922,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
@@ -936,10 +936,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
@@ -947,10 +947,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -961,24 +961,24 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>131</v>
       </c>
       <c r="D15" t="s">
         <v>3</v>
@@ -986,24 +986,24 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
         <v>3</v>
@@ -1011,24 +1011,24 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
         <v>3</v>
@@ -1036,24 +1036,24 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
         <v>3</v>
@@ -1061,24 +1061,24 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
         <v>3</v>
@@ -1086,24 +1086,24 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
         <v>3</v>
@@ -1111,24 +1111,24 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D27" t="s">
         <v>3</v>
@@ -1136,24 +1136,24 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D29" t="s">
         <v>3</v>
@@ -1161,24 +1161,24 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s">
         <v>3</v>
@@ -1186,24 +1186,24 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" t="s">
         <v>3</v>
@@ -1211,24 +1211,24 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
         <v>3</v>
@@ -1236,24 +1236,24 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D37" t="s">
         <v>3</v>
@@ -1261,24 +1261,24 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D39" t="s">
         <v>3</v>
@@ -1286,24 +1286,24 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B40" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B41" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" t="s">
         <v>3</v>
@@ -1311,24 +1311,24 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D43" t="s">
         <v>3</v>
@@ -1336,24 +1336,24 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B44" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B45" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D45" t="s">
         <v>3</v>
@@ -1361,24 +1361,24 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B46" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D47" t="s">
         <v>3</v>
@@ -1386,24 +1386,24 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B48" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B49" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C49" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D49" t="s">
         <v>3</v>
@@ -1411,24 +1411,24 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B50" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C50" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B51" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D51" t="s">
         <v>3</v>
@@ -1436,24 +1436,24 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B52" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C53" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D53" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Corrected Spelling for Cincinnati
</commit_message>
<xml_diff>
--- a/velocity_template.xlsx
+++ b/velocity_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repo\touch_DDGs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F694BAD3-F6FE-49B1-AA8B-C4FE54F21BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81470A9F-4C5C-499A-8C0A-B3469742BD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="57600" windowHeight="15435" xr2:uid="{4C7E114B-A30A-4DC9-9FF5-1565BE38942B}"/>
   </bookViews>
@@ -168,9 +168,6 @@
     <t>Velocity Chula Vista All Staff</t>
   </si>
   <si>
-    <t>Velocity Cincinatti All Staff</t>
-  </si>
-  <si>
     <t>Velocity Cleveland All Staff</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>Velocity Chula Vista Employees</t>
   </si>
   <si>
-    <t>Velocity Cincinatti Employees</t>
-  </si>
-  <si>
     <t>Velocity Cleveland Employees</t>
   </si>
   <si>
@@ -436,6 +430,12 @@
   </si>
   <si>
     <t>velocitycincinnatiemployees</t>
+  </si>
+  <si>
+    <t>Velocity Cincinnati All Staff</t>
+  </si>
+  <si>
+    <t>Velocity Cincinnati Employees</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,7 +889,7 @@
         <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -897,10 +897,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -914,7 +914,7 @@
         <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -922,10 +922,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
@@ -939,7 +939,7 @@
         <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
@@ -947,10 +947,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -961,24 +961,24 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>132</v>
       </c>
       <c r="B14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D15" t="s">
         <v>3</v>
@@ -986,10 +986,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
         <v>21</v>
@@ -997,10 +997,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C17" t="s">
         <v>21</v>
@@ -1011,10 +1011,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
@@ -1022,10 +1022,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C19" t="s">
         <v>23</v>
@@ -1036,10 +1036,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C20" t="s">
         <v>24</v>
@@ -1047,10 +1047,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C21" t="s">
         <v>24</v>
@@ -1061,10 +1061,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
         <v>25</v>
@@ -1072,10 +1072,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
@@ -1086,10 +1086,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C24" t="s">
         <v>26</v>
@@ -1097,10 +1097,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
         <v>26</v>
@@ -1111,10 +1111,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
@@ -1122,10 +1122,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C27" t="s">
         <v>27</v>
@@ -1136,10 +1136,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C28" t="s">
         <v>28</v>
@@ -1147,10 +1147,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
         <v>28</v>
@@ -1161,10 +1161,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C30" t="s">
         <v>29</v>
@@ -1172,10 +1172,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
         <v>29</v>
@@ -1186,10 +1186,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C32" t="s">
         <v>30</v>
@@ -1197,10 +1197,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C33" t="s">
         <v>30</v>
@@ -1211,10 +1211,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C34" t="s">
         <v>31</v>
@@ -1222,10 +1222,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C35" t="s">
         <v>31</v>
@@ -1236,10 +1236,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C36" t="s">
         <v>32</v>
@@ -1247,10 +1247,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C37" t="s">
         <v>32</v>
@@ -1261,10 +1261,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C38" t="s">
         <v>33</v>
@@ -1272,10 +1272,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C39" t="s">
         <v>33</v>
@@ -1286,10 +1286,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B40" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C40" t="s">
         <v>34</v>
@@ -1297,10 +1297,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C41" t="s">
         <v>34</v>
@@ -1311,10 +1311,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B42" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C42" t="s">
         <v>35</v>
@@ -1322,10 +1322,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B43" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
         <v>35</v>
@@ -1336,10 +1336,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B44" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C44" t="s">
         <v>36</v>
@@ -1347,10 +1347,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B45" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C45" t="s">
         <v>36</v>
@@ -1361,10 +1361,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B46" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C46" t="s">
         <v>37</v>
@@ -1372,10 +1372,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B47" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C47" t="s">
         <v>37</v>
@@ -1386,10 +1386,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B48" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C48" t="s">
         <v>38</v>
@@ -1397,10 +1397,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B49" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C49" t="s">
         <v>38</v>
@@ -1411,10 +1411,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B50" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C50" t="s">
         <v>39</v>
@@ -1422,10 +1422,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C51" t="s">
         <v>39</v>
@@ -1436,10 +1436,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B52" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C52" t="s">
         <v>40</v>
@@ -1447,10 +1447,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B53" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C53" t="s">
         <v>40</v>

</xml_diff>